<commit_message>
fix: mapping of fields from properties was   incorrect fix: script was just running on sample_properties instead of full   fake properties file
</commit_message>
<xml_diff>
--- a/data/Field Config.xlsx
+++ b/data/Field Config.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Field Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,17 +493,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Full street address of the property</t>
+          <t>Full street address</t>
         </is>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>123 Main St</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,17 +524,13 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>City name where property is located</t>
+          <t>City name</t>
         </is>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Austin</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -563,17 +555,13 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>State abbreviation (2 characters)</t>
+          <t>State abbreviation</t>
         </is>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -598,17 +586,13 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ZIP code (5 or 9 digits)</t>
+          <t>ZIP code</t>
         </is>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>78701</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -639,11 +623,7 @@
       <c r="F6" t="b">
         <v>0</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Travis County</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -668,17 +648,13 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>GPS latitude coordinate (-90 to 90)</t>
+          <t>GPS latitude</t>
         </is>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>30.267153</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -703,17 +679,13 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>GPS longitude coordinate (-180 to 180)</t>
+          <t>GPS longitude</t>
         </is>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-97.743061</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -738,302 +710,266 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Type of property (Single Family, Condo, etc.)</t>
+          <t>Property type</t>
         </is>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Single Family</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>bedrooms</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>bedrooms</t>
+          <t>address</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>INT</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Number of bedrooms (0-50)</t>
+          <t>Full address</t>
         </is>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bathrooms</t>
+          <t>Street_Address</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>bathrooms</t>
+          <t>address</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Number of bathrooms (can be fractional)</t>
+          <t>Street address</t>
         </is>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2.5</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>square_feet</t>
+          <t>City</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>square_feet</t>
+          <t>city</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>INT</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Living area in square feet</t>
+          <t>City name</t>
         </is>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1800</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lot_size</t>
+          <t>State</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>lot_size</t>
+          <t>state</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lot size in acres</t>
+          <t>State</t>
         </is>
       </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0.25</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>year_built</t>
+          <t>Zip</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>year_built</t>
+          <t>zip_code</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>YEAR</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Year property was built (1800-2100)</t>
+          <t>ZIP</t>
         </is>
       </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>garage_spaces</t>
+          <t>Property_Type</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>garage_spaces</t>
+          <t>property_type</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>INT</t>
+          <t>VARCHAR</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Number of garage parking spaces</t>
+          <t>Property type</t>
         </is>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>basement</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>basement</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>DECIMAL</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Whether property has a basement</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>pool</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>property_details</t>
+          <t>properties</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>pool</t>
+          <t>longitude</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>DECIMAL</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Whether property has a pool</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>fireplace</t>
+          <t>bedrooms</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1043,42 +979,38 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fireplace</t>
+          <t>bedrooms</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>BOOLEAN</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Whether property has a fireplace</t>
+          <t>Number of bedrooms</t>
         </is>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>market_value</t>
+          <t>bathrooms</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>property_valuations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>valuation_amount</t>
+          <t>bathrooms</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1088,67 +1020,59 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Current market value estimate -&gt; Market Value type</t>
+          <t>Number of bathrooms</t>
         </is>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>350000</t>
-        </is>
-      </c>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>tax_assessment</t>
+          <t>square_feet</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>property_valuations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>valuation_amount</t>
+          <t>square_feet</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Tax assessment value -&gt; Tax Assessment type</t>
+          <t>Square footage</t>
         </is>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>280000</t>
-        </is>
-      </c>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>insurance_value</t>
+          <t>lot_size</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>property_valuations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>valuation_amount</t>
+          <t>lot_size</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1158,242 +1082,214 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Insurance replacement value -&gt; Insurance Value type</t>
+          <t>Lot size in acres</t>
         </is>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>380000</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>rental_estimate</t>
+          <t>year_built</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>property_valuations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>valuation_amount</t>
+          <t>year_built</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>YEAR</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Monthly rental income estimate -&gt; Rental Value type</t>
+          <t>Year built</t>
         </is>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>hoa_name</t>
+          <t>garage_spaces</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>hoa_associations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>hoa_name</t>
+          <t>garage_spaces</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VARCHAR</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Name of HOA association</t>
+          <t>Garage spaces</t>
         </is>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Sunset Hills HOA</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>hoa_monthly_fee</t>
+          <t>basement</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>property_hoa_data</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>monthly_fee</t>
+          <t>basement</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Monthly HOA fee amount</t>
+          <t>Has basement</t>
         </is>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>hoa_special_assessment</t>
+          <t>pool</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>property_hoa_data</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>special_assessment</t>
+          <t>pool</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>One-time special assessment amount</t>
+          <t>Has pool</t>
         </is>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>hoa_amenities</t>
+          <t>fireplace</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>property_hoa_data</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>amenities</t>
+          <t>fireplace</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TEXT</t>
+          <t>BOOLEAN</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>List of HOA amenities</t>
+          <t>Has fireplace</t>
         </is>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Pool, Tennis Court, Clubhouse</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>hoa_management</t>
+          <t>Bed</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>hoa_associations</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>management_company</t>
+          <t>bedrooms</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>VARCHAR</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>HOA management company name</t>
+          <t>Bedrooms</t>
         </is>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>ABC Property Management</t>
-        </is>
-      </c>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>kitchen_rehab</t>
+          <t>Bath</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>property_rehab_estimates</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>estimated_cost</t>
+          <t>bathrooms</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1403,157 +1299,726 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Kitchen renovation cost -&gt; Kitchen category</t>
+          <t>Bathrooms</t>
         </is>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>15000</t>
-        </is>
-      </c>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>bathroom_rehab</t>
+          <t>SQFT_Total</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>property_rehab_estimates</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>estimated_cost</t>
+          <t>square_feet</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>INT</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Bathroom renovation cost -&gt; Bathroom category</t>
+          <t>Total square feet</t>
         </is>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>8000</t>
-        </is>
-      </c>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>flooring_cost</t>
+          <t>Year_Built</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>property_rehab_estimates</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>estimated_cost</t>
+          <t>year_built</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>YEAR</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Flooring replacement cost -&gt; Flooring category</t>
+          <t>Year built</t>
         </is>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>roof_repair</t>
+          <t>Pool</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>property_rehab_estimates</t>
+          <t>property_details</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>estimated_cost</t>
+          <t>pool</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>DECIMAL</t>
+          <t>VARCHAR_TO_BOOLEAN</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Roof repair cost -&gt; Roofing category</t>
+          <t>Pool (Yes/No)</t>
         </is>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>12000</t>
-        </is>
-      </c>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>BasementYesNo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>property_details</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>basement</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>VARCHAR_TO_BOOLEAN</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Basement (Yes/No)</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SQFT_Basement</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>property_details</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>square_feet</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>INT</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Basement square feet</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>market_value</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>property_valuations</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>valuation_amount</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Market value -&gt; Market Value type</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>tax_assessment</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>property_valuations</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>valuation_amount</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Tax assessment -&gt; Tax Assessment type</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>insurance_value</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>property_valuations</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>valuation_amount</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Insurance value -&gt; Insurance Value type</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>rental_estimate</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>property_valuations</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>valuation_amount</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Rental estimate -&gt; Rental Value type</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>kitchen_rehab</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Kitchen rehab -&gt; Kitchen category</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>bathroom_rehab</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Bathroom rehab -&gt; Bathroom category</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>flooring_cost</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Flooring cost -&gt; Flooring category</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>roof_repair</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Roof repair -&gt; Roofing category</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>hvac_cost</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>property_rehab_estimates</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>estimated_cost</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>DECIMAL</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>HVAC system cost -&gt; HVAC category</t>
-        </is>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>6000</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>HVAC cost -&gt; HVAC category</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>electrical_work</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Electrical work -&gt; Electrical category</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>plumbing_work</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Plumbing work -&gt; Plumbing category</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>interior_paint</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Interior paint -&gt; Interior category</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>exterior_paint</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>property_rehab_estimates</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>estimated_cost</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Exterior paint -&gt; Exterior category</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>hoa_name</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>hoa_associations</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>hoa_name</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>VARCHAR</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>HOA name</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>hoa_monthly_fee</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>property_hoa_data</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>monthly_fee</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>HOA monthly fee</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>hoa_special_assessment</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>property_hoa_data</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>special_assessment</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>DECIMAL</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>HOA special assessment</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>hoa_amenities</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>property_hoa_data</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>amenities</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>TEXT</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>HOA amenities</t>
+        </is>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>hoa_management</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>hoa_associations</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>management_company</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>VARCHAR</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>HOA management company</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>